<commit_message>
updates to manip check and copy mid echo script
Changed structure and colour for manip check
</commit_message>
<xml_diff>
--- a/Scanning/Manipulation_check/Orders_PILOT/PAR10_RUN01.xlsx
+++ b/Scanning/Manipulation_check/Orders_PILOT/PAR10_RUN01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Trial</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Face22_L.png</t>
-  </si>
-  <si>
-    <t>Response.png</t>
   </si>
   <si>
     <t>2D</t>
@@ -419,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F41"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +492,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -509,19 +506,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -529,19 +526,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -549,19 +546,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -569,19 +566,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -589,19 +586,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -609,39 +606,30 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -649,19 +637,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -669,19 +657,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -689,19 +677,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -709,19 +697,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -729,50 +717,50 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -780,19 +768,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -800,19 +788,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -820,19 +808,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -840,19 +828,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -860,372 +848,21 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>17</v>
-      </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>18</v>
-      </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>